<commit_message>
TestNG throwing test ignored error when Dataprovider annotation is used
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pboopathi/Documents/Priya/PETproject/Selenium_POM_Project/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51352C73-FA2E-ED45-B77B-14DF0E0EF106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8CCEA-B0A6-7245-8797-D978CE37D345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -490,6 +490,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,9 +554,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -901,7 +917,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -910,26 +926,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>